<commit_message>
Remove status column and change sorting on Imms forecast for AB#14631
</commit_message>
<xml_diff>
--- a/Apps/GatewayApi/src/Assets/Templates/DependentImmunizationReport.xlsx
+++ b/Apps/GatewayApi/src/Assets/Templates/DependentImmunizationReport.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brianjang/Repo/healthgateway/Apps/WebClient/src/Server/Assets/Templates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rayking29/Projects/healthgateway/Apps/GatewayApi/src/Assets/Templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8D24AC1-A480-F941-B901-95B0980F4F5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C14BE48B-C958-BF4B-BDAB-2549472FC2D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-40280" yWindow="4340" windowWidth="28040" windowHeight="17440" xr2:uid="{F605F369-0C71-414E-B75C-5C18C8076E19}"/>
+    <workbookView xWindow="8340" yWindow="1920" windowWidth="28040" windowHeight="17440" xr2:uid="{F605F369-0C71-414E-B75C-5C18C8076E19}"/>
   </bookViews>
   <sheets>
     <sheet name="Immunizations" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
   <si>
     <t>Date</t>
   </si>
@@ -85,16 +85,7 @@
     <t>Due Date</t>
   </si>
   <si>
-    <t>Status</t>
-  </si>
-  <si>
     <t>{d.recommendations[i+1].due_date}</t>
-  </si>
-  <si>
-    <t>{d.recommendations[i].status}</t>
-  </si>
-  <si>
-    <t>{d.recommendations[i+1].status}</t>
   </si>
   <si>
     <t>{d.recommendations[i].due_date}</t>
@@ -178,11 +169,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -204,7 +194,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -492,7 +482,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -503,7 +493,7 @@
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -515,12 +505,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -542,48 +532,48 @@
       <c r="H2" s="1"/>
     </row>
     <row r="3" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B3" t="s">
         <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E3" t="s">
         <v>9</v>
       </c>
       <c r="F3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B4" t="s">
         <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E4" t="s">
         <v>11</v>
       </c>
       <c r="F4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="21" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>21</v>
+      <c r="A7" s="3" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
@@ -593,19 +583,14 @@
       <c r="B8" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>16</v>
-      </c>
+      <c r="C8" s="1"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>20</v>
-      </c>
-      <c r="C9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
@@ -613,10 +598,7 @@
         <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Remove status column and change sorting on Imms forecast for AB#14631 (#4604)
</commit_message>
<xml_diff>
--- a/Apps/GatewayApi/src/Assets/Templates/DependentImmunizationReport.xlsx
+++ b/Apps/GatewayApi/src/Assets/Templates/DependentImmunizationReport.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brianjang/Repo/healthgateway/Apps/WebClient/src/Server/Assets/Templates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rayking29/Projects/healthgateway/Apps/GatewayApi/src/Assets/Templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8D24AC1-A480-F941-B901-95B0980F4F5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C14BE48B-C958-BF4B-BDAB-2549472FC2D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-40280" yWindow="4340" windowWidth="28040" windowHeight="17440" xr2:uid="{F605F369-0C71-414E-B75C-5C18C8076E19}"/>
+    <workbookView xWindow="8340" yWindow="1920" windowWidth="28040" windowHeight="17440" xr2:uid="{F605F369-0C71-414E-B75C-5C18C8076E19}"/>
   </bookViews>
   <sheets>
     <sheet name="Immunizations" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
   <si>
     <t>Date</t>
   </si>
@@ -85,16 +85,7 @@
     <t>Due Date</t>
   </si>
   <si>
-    <t>Status</t>
-  </si>
-  <si>
     <t>{d.recommendations[i+1].due_date}</t>
-  </si>
-  <si>
-    <t>{d.recommendations[i].status}</t>
-  </si>
-  <si>
-    <t>{d.recommendations[i+1].status}</t>
   </si>
   <si>
     <t>{d.recommendations[i].due_date}</t>
@@ -178,11 +169,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -204,7 +194,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -492,7 +482,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -503,7 +493,7 @@
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -515,12 +505,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -542,48 +532,48 @@
       <c r="H2" s="1"/>
     </row>
     <row r="3" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B3" t="s">
         <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E3" t="s">
         <v>9</v>
       </c>
       <c r="F3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B4" t="s">
         <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E4" t="s">
         <v>11</v>
       </c>
       <c r="F4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="21" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>21</v>
+      <c r="A7" s="3" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
@@ -593,19 +583,14 @@
       <c r="B8" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>16</v>
-      </c>
+      <c r="C8" s="1"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>20</v>
-      </c>
-      <c r="C9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
@@ -613,10 +598,7 @@
         <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>